<commit_message>
feat(fe-piattaforma): fe updates 09222022
</commit_message>
<xml_diff>
--- a/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
+++ b/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niccolo.valente/Documents/Projects/MITD/public/assets/entity_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/paolo_zappa_accenture_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47660BF-639F-8545-85D2-7D629E515BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{6A440FFC-9321-498E-9917-382FC606348B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86C4259A-79C7-474F-9883-8EF0AE84A046}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19720" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="290">
   <si>
     <t>CodiceFiscale</t>
   </si>
@@ -85,57 +85,12 @@
     <t>Telefono</t>
   </si>
   <si>
-    <t>Paolino</t>
-  </si>
-  <si>
-    <t>Maldini</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>DIPLOMA</t>
-  </si>
-  <si>
-    <t>ITA</t>
-  </si>
-  <si>
-    <t>Roma</t>
-  </si>
-  <si>
-    <t>pao.maldini@emial.com</t>
-  </si>
-  <si>
-    <t>PROVAZ28B99Z993X</t>
-  </si>
-  <si>
-    <t>PROVAQ18A12T561I</t>
-  </si>
-  <si>
-    <t>Enzo</t>
-  </si>
-  <si>
-    <t>Ferrari</t>
-  </si>
-  <si>
-    <t>enzo.ferrari@emial.com</t>
-  </si>
-  <si>
-    <t>FRCRSS55A12B335Y</t>
-  </si>
-  <si>
-    <t>FRANCO</t>
-  </si>
-  <si>
-    <t>ROSSINO</t>
-  </si>
-  <si>
     <t>Carta di Identità</t>
   </si>
   <si>
-    <t>3434434343</t>
-  </si>
-  <si>
     <t>Licenza media inferiore / Scuola secondaria di I grado (3 anni)</t>
   </si>
   <si>
@@ -938,6 +893,18 @@
   </si>
   <si>
     <t>+263</t>
+  </si>
+  <si>
+    <t>1953</t>
+  </si>
+  <si>
+    <t>MARCO</t>
+  </si>
+  <si>
+    <t>BICCI</t>
+  </si>
+  <si>
+    <t>BCCMRC53A12TY55Y</t>
   </si>
 </sst>
 </file>
@@ -982,9 +949,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -1306,29 +1272,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8BEB98-427E-496B-B7BD-F71A2D02D0A0}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1378,178 +1334,502 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2">
-        <v>1982</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2">
-        <v>39</v>
-      </c>
-      <c r="O2">
-        <v>3366998810</v>
-      </c>
-      <c r="P2">
-        <v>2252365</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="O2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="P2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3">
-        <v>1983</v>
-      </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3">
-        <v>39</v>
-      </c>
-      <c r="O3">
-        <v>3206788123</v>
-      </c>
-      <c r="P3">
-        <v>2569861</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1955</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>41</v>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="Q101">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{E73C9308-4C24-4200-8289-D1CFAC6DEB17}"/>
-    <hyperlink ref="M3" r:id="rId2" xr:uid="{50F572A2-E509-4727-A1E9-1EEB641D8604}"/>
-    <hyperlink ref="M4" r:id="rId3" xr:uid="{F351616E-F65B-4FE8-A381-7F8849054211}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{F351616E-F65B-4FE8-A381-7F8849054211}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="G2" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CD1938C-E620-418E-AE83-63A444E6FE08}">
           <x14:formula1>
             <xm:f>valori!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L4</xm:sqref>
+          <xm:sqref>L2:L101</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C0FA6E0-F7E0-4DC8-B25F-A72B4D311A58}">
           <x14:formula1>
             <xm:f>valori!$C$2:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H4</xm:sqref>
+          <xm:sqref>H2:H100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AE43BD5-0167-4321-B099-FDE2FB6A1933}">
           <x14:formula1>
             <xm:f>valori!$D$2:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I4</xm:sqref>
+          <xm:sqref>I2:I100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{982C8DCC-435C-421D-8EA1-21A053C25223}">
           <x14:formula1>
             <xm:f>valori!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J4</xm:sqref>
+          <xm:sqref>J2:J100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECD8C6CC-EDBD-48A8-A51C-9053D522AE1F}">
+          <x14:formula1>
+            <xm:f>valori!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCF0EE29-51E8-4E2A-B6CD-216BA845A309}">
+          <x14:formula1>
+            <xm:f>valori!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F101</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50897BB4-255D-43E6-8928-804484AA2B28}">
+          <x14:formula1>
+            <xm:f>valori!$G$2:$G$237</xm:f>
+          </x14:formula1>
+          <xm:sqref>N2:N101</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1561,21 +1841,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA2305A-781D-4ABB-83F9-A2AAD4F5F6E0}">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A218" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" customWidth="1"/>
+    <col min="6" max="6" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1583,7 +1863,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1592,1295 +1872,1295 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C6" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D6" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="5" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D7" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D8" t="s">
         <v>55</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="5" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D9" t="s">
         <v>58</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
         <v>62</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
         <v>66</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="5" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G15" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="5" t="s">
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G18" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G19" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="5" t="s">
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G20" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="5" t="s">
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G22" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G23" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="5" t="s">
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G24" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G25" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="5" t="s">
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G26" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="5" t="s">
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G28" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="5" t="s">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G29" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G15" s="5" t="s">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G30" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G16" s="5" t="s">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G31" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" s="5" t="s">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G32" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G18" s="5" t="s">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G33" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G19" s="5" t="s">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G34" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G35" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G20" s="5" t="s">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G36" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G21" s="2" t="s">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G37" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G22" s="5" t="s">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G38" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G23" s="5" t="s">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G39" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G40" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G24" s="5" t="s">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G41" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G25" s="5" t="s">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G42" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G26" s="5" t="s">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G43" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G27" s="5" t="s">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G44" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G28" s="5" t="s">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G45" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G29" s="5" t="s">
+    <row r="46" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G46" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G30" s="5" t="s">
+    <row r="47" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G47" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G31" s="5" t="s">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G48" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G32" s="5" t="s">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G49" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G33" s="5" t="s">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G50" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G34" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G35" s="5" t="s">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G51" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G36" s="5" t="s">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G52" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G37" s="5" t="s">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G53" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G38" s="5" t="s">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G54" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G39" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G40" s="5" t="s">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G55" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G41" s="5" t="s">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G56" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G42" s="5" t="s">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G57" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="5" t="s">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G58" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G44" s="5" t="s">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G59" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G45" s="5" t="s">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G60" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G46" s="5" t="s">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G61" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G47" s="5" t="s">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G62" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G48" s="5" t="s">
+    <row r="63" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G63" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G49" s="5" t="s">
+    <row r="64" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G64" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G50" s="5" t="s">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G65" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G51" s="5" t="s">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G66" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G52" s="5" t="s">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G67" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G53" s="5" t="s">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G68" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G54" s="5" t="s">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G69" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G55" s="5" t="s">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G70" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G56" s="5" t="s">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G71" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G57" s="5" t="s">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G72" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G58" s="5" t="s">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G73" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G59" s="5" t="s">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G74" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G60" s="5" t="s">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G75" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G61" s="5" t="s">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G76" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G62" s="5" t="s">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G77" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G63" s="5" t="s">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G78" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G64" s="5" t="s">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G79" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G65" s="5" t="s">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G80" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G66" s="5" t="s">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G81" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G67" s="5" t="s">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G82" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G68" s="5" t="s">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G83" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G69" s="5" t="s">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G84" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G70" s="5" t="s">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G85" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G71" s="5" t="s">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G86" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G72" s="5" t="s">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G87" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G73" s="5" t="s">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G88" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G74" s="5" t="s">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G89" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G75" s="5" t="s">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G90" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G76" s="5" t="s">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G91" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G77" s="5" t="s">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G92" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G78" s="5" t="s">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G93" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G79" s="5" t="s">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G94" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G80" s="5" t="s">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G95" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G81" s="5" t="s">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G96" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G82" s="5" t="s">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G97" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G83" s="5" t="s">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G98" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G84" s="5" t="s">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G99" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G85" s="5" t="s">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G100" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G86" s="5" t="s">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G101" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G87" s="5" t="s">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G102" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G88" s="5" t="s">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G103" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G89" s="5" t="s">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G104" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G90" s="5" t="s">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G105" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G91" s="5" t="s">
+    <row r="106" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G106" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G92" s="5" t="s">
+    <row r="107" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G107" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G93" s="5" t="s">
+    <row r="108" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G108" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G94" s="5" t="s">
+    <row r="109" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G109" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G95" s="5" t="s">
+    <row r="110" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G110" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G96" s="5" t="s">
+    <row r="111" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G111" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G97" s="5" t="s">
+    <row r="112" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G112" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G98" s="5" t="s">
+    <row r="113" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G113" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G99" s="5" t="s">
+    <row r="114" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G114" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G100" s="5" t="s">
+    <row r="115" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G115" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G101" s="5" t="s">
+    <row r="116" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G116" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G102" s="5" t="s">
+    <row r="117" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G117" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G103" s="5" t="s">
+    <row r="118" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G118" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G104" s="5" t="s">
+    <row r="119" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G119" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G105" s="5" t="s">
+    <row r="120" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G120" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G106" s="5" t="s">
+    <row r="121" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G121" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G107" s="5" t="s">
+    <row r="122" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G122" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G108" s="5" t="s">
+    <row r="123" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G123" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G109" s="5" t="s">
+    <row r="124" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G124" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G110" s="5" t="s">
+    <row r="125" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G125" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G111" s="5" t="s">
+    <row r="126" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G126" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G112" s="5" t="s">
+    <row r="127" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G127" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G113" s="5" t="s">
+    <row r="128" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G128" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G114" s="5" t="s">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G129" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G115" s="5" t="s">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G130" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="131" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G131" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G116" s="5" t="s">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G132" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G117" s="5" t="s">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G133" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G118" s="5" t="s">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G134" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G119" s="5" t="s">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G135" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G120" s="5" t="s">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G136" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G121" s="5" t="s">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G137" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G122" s="5" t="s">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G138" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G123" s="5" t="s">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G139" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G124" s="5" t="s">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G140" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G125" s="5" t="s">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G141" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G126" s="5" t="s">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G142" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G127" s="5" t="s">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G143" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G128" s="5" t="s">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G144" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G129" s="5" t="s">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G145" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G130" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G131" s="5" t="s">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G146" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G132" s="5" t="s">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G147" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G133" s="5" t="s">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G148" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G134" s="5" t="s">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G149" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G135" s="5" t="s">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G150" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G136" s="5" t="s">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G151" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G137" s="5" t="s">
+    <row r="152" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G152" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G138" s="5" t="s">
+    <row r="153" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G153" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G139" s="5" t="s">
+    <row r="154" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G154" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="155" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G155" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G140" s="5" t="s">
+    <row r="156" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G156" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G141" s="5" t="s">
+    <row r="157" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G157" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G142" s="5" t="s">
+    <row r="158" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G158" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G143" s="5" t="s">
+    <row r="159" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G159" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G144" s="5" t="s">
+    <row r="160" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G160" s="4" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G145" s="5" t="s">
+    <row r="161" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G161" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G146" s="5" t="s">
+    <row r="162" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G162" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G147" s="5" t="s">
+    <row r="163" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G163" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G148" s="5" t="s">
+    <row r="164" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G164" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G149" s="5" t="s">
+    <row r="165" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G165" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G150" s="5" t="s">
+    <row r="166" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G166" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G151" s="5" t="s">
+    <row r="167" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G167" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G152" s="5" t="s">
+    <row r="168" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G168" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G153" s="5" t="s">
+    <row r="169" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G169" s="4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G154" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G155" s="5" t="s">
+    <row r="170" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G170" s="4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G156" s="5" t="s">
+    <row r="171" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G171" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G157" s="5" t="s">
+    <row r="172" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G172" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G158" s="5" t="s">
+    <row r="173" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G173" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G159" s="5" t="s">
+    <row r="174" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G174" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G160" s="5" t="s">
+    <row r="175" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G175" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G161" s="5" t="s">
+    <row r="176" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G176" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G162" s="5" t="s">
+    <row r="177" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G177" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G163" s="5" t="s">
+    <row r="178" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G178" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G164" s="5" t="s">
+    <row r="179" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G179" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G165" s="5" t="s">
+    <row r="180" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G180" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G166" s="5" t="s">
+    <row r="181" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G181" s="4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G167" s="5" t="s">
+    <row r="182" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G182" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G168" s="5" t="s">
+    <row r="183" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G183" s="4" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G169" s="5" t="s">
+    <row r="184" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G184" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G170" s="5" t="s">
+    <row r="185" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G185" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G171" s="5" t="s">
+    <row r="186" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G186" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G172" s="5" t="s">
+    <row r="187" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G187" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G173" s="5" t="s">
+    <row r="188" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G188" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G174" s="5" t="s">
+    <row r="189" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G189" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G175" s="5" t="s">
+    <row r="190" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G190" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G176" s="5" t="s">
+    <row r="191" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G191" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G177" s="5" t="s">
+    <row r="192" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G192" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G178" s="5" t="s">
+    <row r="193" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G193" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G179" s="5" t="s">
+    <row r="194" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G194" s="4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G180" s="5" t="s">
+    <row r="195" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G195" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G181" s="5" t="s">
+    <row r="196" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G196" s="4" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G182" s="5" t="s">
+    <row r="197" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G197" s="4" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G183" s="5" t="s">
+    <row r="198" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G198" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G184" s="5" t="s">
+    <row r="199" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G199" s="4" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G185" s="5" t="s">
+    <row r="200" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G200" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G186" s="5" t="s">
+    <row r="201" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G201" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G187" s="5" t="s">
+    <row r="202" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G202" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G188" s="5" t="s">
+    <row r="203" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G203" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G189" s="5" t="s">
+    <row r="204" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G204" s="4" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G190" s="5" t="s">
+    <row r="205" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G205" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G191" s="5" t="s">
+    <row r="206" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G206" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G192" s="5" t="s">
+    <row r="207" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G207" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G193" s="5" t="s">
+    <row r="208" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G208" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G194" s="5" t="s">
+    <row r="209" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G209" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G195" s="5" t="s">
+    <row r="210" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G210" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G196" s="5" t="s">
+    <row r="211" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G211" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G197" s="5" t="s">
+    <row r="212" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G212" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G198" s="5" t="s">
+    <row r="213" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G213" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G199" s="5" t="s">
+    <row r="214" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G214" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G200" s="5" t="s">
+    <row r="215" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G215" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G201" s="5" t="s">
+    <row r="216" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G216" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G202" s="5" t="s">
+    <row r="217" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G217" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G203" s="5" t="s">
+    <row r="218" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G218" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G204" s="5" t="s">
+    <row r="219" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G219" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G205" s="5" t="s">
+    <row r="220" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G220" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="221" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G221" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G206" s="5" t="s">
+    <row r="222" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G222" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G207" s="5" t="s">
+    <row r="223" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G223" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G208" s="5" t="s">
+    <row r="224" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G224" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G209" s="5" t="s">
+    <row r="225" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G225" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G210" s="5" t="s">
+    <row r="226" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G226" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G211" s="5" t="s">
+    <row r="227" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G227" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G212" s="5" t="s">
+    <row r="228" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G228" s="4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G213" s="5" t="s">
+    <row r="229" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G229" s="4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G214" s="5" t="s">
+    <row r="230" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G230" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G215" s="5" t="s">
+    <row r="231" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G231" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G216" s="5" t="s">
+    <row r="232" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G232" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G217" s="5" t="s">
+    <row r="233" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G233" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G234" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G218" s="5" t="s">
+    <row r="235" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G235" s="4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G219" s="5" t="s">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G236" s="4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G220" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G221" s="5" t="s">
+    <row r="237" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G237" s="4" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G222" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G223" s="5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G224" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G225" s="5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G226" s="5" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G227" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G228" s="5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G229" s="5" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G230" s="5" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G231" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G232" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G233" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G234" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G235" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G236" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G237" s="5" t="s">
-        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2895,15 +3175,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100203199D83812C2499E49CC0C3E7DE06C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2f8823872235ddf1d1c55d8837f3ca9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="631437c1-70b7-41ea-97e4-3973abe7cce0" xmlns:ns4="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="116abd7a6875440f2166ad9e25254cea" ns3:_="" ns4:_="">
     <xsd:import namespace="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
@@ -3112,6 +3383,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F8F7E8B-C071-4DC9-A2E9-BDAF31C19E75}">
   <ds:schemaRefs>
@@ -3130,14 +3410,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{214CF277-9889-499D-8A02-51B999F78EC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3154,4 +3426,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(fe-piattaforma): fe updates 09232022
</commit_message>
<xml_diff>
--- a/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
+++ b/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niccolo.valente/Documents/Projects/MITD/public/assets/entity_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.zappa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47660BF-639F-8545-85D2-7D629E515BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AA2B79-2828-4DB9-8E58-E32F53D08181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19720" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
-    <sheet name="valori" sheetId="3" r:id="rId2"/>
+    <sheet name="valori" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="290">
   <si>
     <t>CodiceFiscale</t>
   </si>
@@ -85,57 +85,12 @@
     <t>Telefono</t>
   </si>
   <si>
-    <t>Paolino</t>
-  </si>
-  <si>
-    <t>Maldini</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>DIPLOMA</t>
-  </si>
-  <si>
-    <t>ITA</t>
-  </si>
-  <si>
-    <t>Roma</t>
-  </si>
-  <si>
-    <t>pao.maldini@emial.com</t>
-  </si>
-  <si>
-    <t>PROVAZ28B99Z993X</t>
-  </si>
-  <si>
-    <t>PROVAQ18A12T561I</t>
-  </si>
-  <si>
-    <t>Enzo</t>
-  </si>
-  <si>
-    <t>Ferrari</t>
-  </si>
-  <si>
-    <t>enzo.ferrari@emial.com</t>
-  </si>
-  <si>
-    <t>FRCRSS55A12B335Y</t>
-  </si>
-  <si>
-    <t>FRANCO</t>
-  </si>
-  <si>
-    <t>ROSSINO</t>
-  </si>
-  <si>
     <t>Carta di Identità</t>
   </si>
   <si>
-    <t>3434434343</t>
-  </si>
-  <si>
     <t>Licenza media inferiore / Scuola secondaria di I grado (3 anni)</t>
   </si>
   <si>
@@ -938,6 +893,18 @@
   </si>
   <si>
     <t>+263</t>
+  </si>
+  <si>
+    <t>1953</t>
+  </si>
+  <si>
+    <t>MARCO</t>
+  </si>
+  <si>
+    <t>BICCI</t>
+  </si>
+  <si>
+    <t>BCCMRC53A16T995Y</t>
   </si>
 </sst>
 </file>
@@ -982,9 +949,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -1306,29 +1272,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8BEB98-427E-496B-B7BD-F71A2D02D0A0}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1378,178 +1334,502 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2">
-        <v>1982</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2">
-        <v>39</v>
-      </c>
-      <c r="O2">
-        <v>3366998810</v>
-      </c>
-      <c r="P2">
-        <v>2252365</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="O2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="P2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3">
-        <v>1983</v>
-      </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3">
-        <v>39</v>
-      </c>
-      <c r="O3">
-        <v>3206788123</v>
-      </c>
-      <c r="P3">
-        <v>2569861</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1955</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>41</v>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="8:17" x14ac:dyDescent="0.35">
+      <c r="Q101">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{E73C9308-4C24-4200-8289-D1CFAC6DEB17}"/>
-    <hyperlink ref="M3" r:id="rId2" xr:uid="{50F572A2-E509-4727-A1E9-1EEB641D8604}"/>
-    <hyperlink ref="M4" r:id="rId3" xr:uid="{F351616E-F65B-4FE8-A381-7F8849054211}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{F351616E-F65B-4FE8-A381-7F8849054211}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="G2" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CD1938C-E620-418E-AE83-63A444E6FE08}">
           <x14:formula1>
             <xm:f>valori!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L4</xm:sqref>
+          <xm:sqref>L2:L101</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C0FA6E0-F7E0-4DC8-B25F-A72B4D311A58}">
           <x14:formula1>
             <xm:f>valori!$C$2:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H4</xm:sqref>
+          <xm:sqref>H2:H100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AE43BD5-0167-4321-B099-FDE2FB6A1933}">
           <x14:formula1>
             <xm:f>valori!$D$2:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I4</xm:sqref>
+          <xm:sqref>I2:I100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{982C8DCC-435C-421D-8EA1-21A053C25223}">
           <x14:formula1>
             <xm:f>valori!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J4</xm:sqref>
+          <xm:sqref>J2:J100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECD8C6CC-EDBD-48A8-A51C-9053D522AE1F}">
+          <x14:formula1>
+            <xm:f>valori!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCF0EE29-51E8-4E2A-B6CD-216BA845A309}">
+          <x14:formula1>
+            <xm:f>valori!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F101</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50897BB4-255D-43E6-8928-804484AA2B28}">
+          <x14:formula1>
+            <xm:f>valori!$G$2:$G$237</xm:f>
+          </x14:formula1>
+          <xm:sqref>N2:N101</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1561,21 +1841,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA2305A-781D-4ABB-83F9-A2AAD4F5F6E0}">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A218" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" customWidth="1"/>
+    <col min="6" max="6" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1583,7 +1863,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1592,1295 +1872,1295 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C6" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D6" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="5" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D7" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D8" t="s">
         <v>55</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="5" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D9" t="s">
         <v>58</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
         <v>62</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
         <v>66</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="5" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G15" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="5" t="s">
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G18" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G19" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="5" t="s">
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G20" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="5" t="s">
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G22" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G23" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="5" t="s">
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G24" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G25" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="5" t="s">
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G26" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="5" t="s">
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G28" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="5" t="s">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G29" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G15" s="5" t="s">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G30" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G16" s="5" t="s">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G31" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" s="5" t="s">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G32" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G18" s="5" t="s">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G33" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G19" s="5" t="s">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G34" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G35" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G20" s="5" t="s">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G36" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G21" s="2" t="s">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G37" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G22" s="5" t="s">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G38" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G23" s="5" t="s">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G39" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G40" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G24" s="5" t="s">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G41" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G25" s="5" t="s">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G42" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G26" s="5" t="s">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G43" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G27" s="5" t="s">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G44" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G28" s="5" t="s">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G45" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G29" s="5" t="s">
+    <row r="46" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G46" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G30" s="5" t="s">
+    <row r="47" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G47" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G31" s="5" t="s">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G48" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G32" s="5" t="s">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G49" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G33" s="5" t="s">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G50" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G34" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G35" s="5" t="s">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G51" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G36" s="5" t="s">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G52" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G37" s="5" t="s">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G53" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G38" s="5" t="s">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G54" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G39" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G40" s="5" t="s">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G55" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G41" s="5" t="s">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G56" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G42" s="5" t="s">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G57" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="5" t="s">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G58" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G44" s="5" t="s">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G59" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G45" s="5" t="s">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G60" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G46" s="5" t="s">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G61" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G47" s="5" t="s">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G62" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G48" s="5" t="s">
+    <row r="63" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G63" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G49" s="5" t="s">
+    <row r="64" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G64" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G50" s="5" t="s">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G65" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G51" s="5" t="s">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G66" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G52" s="5" t="s">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G67" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G53" s="5" t="s">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G68" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G54" s="5" t="s">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G69" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G55" s="5" t="s">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G70" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G56" s="5" t="s">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G71" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G57" s="5" t="s">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G72" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G58" s="5" t="s">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G73" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G59" s="5" t="s">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G74" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G60" s="5" t="s">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G75" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G61" s="5" t="s">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G76" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G62" s="5" t="s">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G77" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G63" s="5" t="s">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G78" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G64" s="5" t="s">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G79" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G65" s="5" t="s">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G80" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G66" s="5" t="s">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G81" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G67" s="5" t="s">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G82" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G68" s="5" t="s">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G83" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G69" s="5" t="s">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G84" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G70" s="5" t="s">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G85" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G71" s="5" t="s">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G86" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G72" s="5" t="s">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G87" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G73" s="5" t="s">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G88" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G74" s="5" t="s">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G89" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G75" s="5" t="s">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G90" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G76" s="5" t="s">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G91" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G77" s="5" t="s">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G92" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G78" s="5" t="s">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G93" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G79" s="5" t="s">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G94" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G80" s="5" t="s">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G95" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G81" s="5" t="s">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G96" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G82" s="5" t="s">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G97" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G83" s="5" t="s">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G98" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G84" s="5" t="s">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G99" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G85" s="5" t="s">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G100" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G86" s="5" t="s">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G101" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G87" s="5" t="s">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G102" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G88" s="5" t="s">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G103" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G89" s="5" t="s">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G104" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G90" s="5" t="s">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G105" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G91" s="5" t="s">
+    <row r="106" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G106" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G92" s="5" t="s">
+    <row r="107" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G107" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G93" s="5" t="s">
+    <row r="108" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G108" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G94" s="5" t="s">
+    <row r="109" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G109" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G95" s="5" t="s">
+    <row r="110" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G110" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G96" s="5" t="s">
+    <row r="111" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G111" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G97" s="5" t="s">
+    <row r="112" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G112" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G98" s="5" t="s">
+    <row r="113" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G113" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G99" s="5" t="s">
+    <row r="114" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G114" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G100" s="5" t="s">
+    <row r="115" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G115" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G101" s="5" t="s">
+    <row r="116" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G116" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G102" s="5" t="s">
+    <row r="117" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G117" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G103" s="5" t="s">
+    <row r="118" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G118" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G104" s="5" t="s">
+    <row r="119" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G119" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G105" s="5" t="s">
+    <row r="120" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G120" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G106" s="5" t="s">
+    <row r="121" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G121" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G107" s="5" t="s">
+    <row r="122" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G122" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G108" s="5" t="s">
+    <row r="123" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G123" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G109" s="5" t="s">
+    <row r="124" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G124" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G110" s="5" t="s">
+    <row r="125" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G125" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G111" s="5" t="s">
+    <row r="126" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G126" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G112" s="5" t="s">
+    <row r="127" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G127" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G113" s="5" t="s">
+    <row r="128" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G128" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G114" s="5" t="s">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G129" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G115" s="5" t="s">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G130" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="131" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G131" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G116" s="5" t="s">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G132" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G117" s="5" t="s">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G133" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G118" s="5" t="s">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G134" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G119" s="5" t="s">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G135" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G120" s="5" t="s">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G136" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G121" s="5" t="s">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G137" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G122" s="5" t="s">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G138" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G123" s="5" t="s">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G139" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G124" s="5" t="s">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G140" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G125" s="5" t="s">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G141" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G126" s="5" t="s">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G142" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G127" s="5" t="s">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G143" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G128" s="5" t="s">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G144" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G129" s="5" t="s">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G145" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G130" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G131" s="5" t="s">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G146" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G132" s="5" t="s">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G147" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G133" s="5" t="s">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G148" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G134" s="5" t="s">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G149" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G135" s="5" t="s">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G150" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G136" s="5" t="s">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G151" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G137" s="5" t="s">
+    <row r="152" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G152" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G138" s="5" t="s">
+    <row r="153" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G153" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G139" s="5" t="s">
+    <row r="154" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G154" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="155" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G155" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G140" s="5" t="s">
+    <row r="156" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G156" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G141" s="5" t="s">
+    <row r="157" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G157" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G142" s="5" t="s">
+    <row r="158" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G158" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G143" s="5" t="s">
+    <row r="159" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G159" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G144" s="5" t="s">
+    <row r="160" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G160" s="4" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G145" s="5" t="s">
+    <row r="161" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G161" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G146" s="5" t="s">
+    <row r="162" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G162" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G147" s="5" t="s">
+    <row r="163" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G163" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G148" s="5" t="s">
+    <row r="164" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G164" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G149" s="5" t="s">
+    <row r="165" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G165" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G150" s="5" t="s">
+    <row r="166" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G166" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G151" s="5" t="s">
+    <row r="167" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G167" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G152" s="5" t="s">
+    <row r="168" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G168" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G153" s="5" t="s">
+    <row r="169" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G169" s="4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G154" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G155" s="5" t="s">
+    <row r="170" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G170" s="4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G156" s="5" t="s">
+    <row r="171" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G171" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G157" s="5" t="s">
+    <row r="172" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G172" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G158" s="5" t="s">
+    <row r="173" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G173" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G159" s="5" t="s">
+    <row r="174" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G174" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G160" s="5" t="s">
+    <row r="175" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G175" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G161" s="5" t="s">
+    <row r="176" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G176" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G162" s="5" t="s">
+    <row r="177" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G177" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G163" s="5" t="s">
+    <row r="178" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G178" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G164" s="5" t="s">
+    <row r="179" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G179" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G165" s="5" t="s">
+    <row r="180" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G180" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G166" s="5" t="s">
+    <row r="181" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G181" s="4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G167" s="5" t="s">
+    <row r="182" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G182" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G168" s="5" t="s">
+    <row r="183" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G183" s="4" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G169" s="5" t="s">
+    <row r="184" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G184" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G170" s="5" t="s">
+    <row r="185" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G185" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G171" s="5" t="s">
+    <row r="186" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G186" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G172" s="5" t="s">
+    <row r="187" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G187" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G173" s="5" t="s">
+    <row r="188" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G188" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G174" s="5" t="s">
+    <row r="189" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G189" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G175" s="5" t="s">
+    <row r="190" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G190" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G176" s="5" t="s">
+    <row r="191" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G191" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G177" s="5" t="s">
+    <row r="192" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G192" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G178" s="5" t="s">
+    <row r="193" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G193" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G179" s="5" t="s">
+    <row r="194" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G194" s="4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G180" s="5" t="s">
+    <row r="195" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G195" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G181" s="5" t="s">
+    <row r="196" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G196" s="4" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G182" s="5" t="s">
+    <row r="197" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G197" s="4" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G183" s="5" t="s">
+    <row r="198" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G198" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G184" s="5" t="s">
+    <row r="199" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G199" s="4" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G185" s="5" t="s">
+    <row r="200" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G200" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G186" s="5" t="s">
+    <row r="201" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G201" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G187" s="5" t="s">
+    <row r="202" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G202" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G188" s="5" t="s">
+    <row r="203" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G203" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G189" s="5" t="s">
+    <row r="204" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G204" s="4" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G190" s="5" t="s">
+    <row r="205" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G205" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G191" s="5" t="s">
+    <row r="206" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G206" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G192" s="5" t="s">
+    <row r="207" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G207" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G193" s="5" t="s">
+    <row r="208" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G208" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G194" s="5" t="s">
+    <row r="209" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G209" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G195" s="5" t="s">
+    <row r="210" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G210" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G196" s="5" t="s">
+    <row r="211" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G211" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G197" s="5" t="s">
+    <row r="212" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G212" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G198" s="5" t="s">
+    <row r="213" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G213" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G199" s="5" t="s">
+    <row r="214" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G214" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G200" s="5" t="s">
+    <row r="215" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G215" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G201" s="5" t="s">
+    <row r="216" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G216" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G202" s="5" t="s">
+    <row r="217" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G217" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G203" s="5" t="s">
+    <row r="218" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G218" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G204" s="5" t="s">
+    <row r="219" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G219" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G205" s="5" t="s">
+    <row r="220" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G220" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="221" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G221" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G206" s="5" t="s">
+    <row r="222" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G222" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G207" s="5" t="s">
+    <row r="223" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G223" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G208" s="5" t="s">
+    <row r="224" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G224" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G209" s="5" t="s">
+    <row r="225" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G225" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G210" s="5" t="s">
+    <row r="226" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G226" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G211" s="5" t="s">
+    <row r="227" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G227" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G212" s="5" t="s">
+    <row r="228" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G228" s="4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G213" s="5" t="s">
+    <row r="229" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G229" s="4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G214" s="5" t="s">
+    <row r="230" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G230" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G215" s="5" t="s">
+    <row r="231" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G231" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G216" s="5" t="s">
+    <row r="232" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G232" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G217" s="5" t="s">
+    <row r="233" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G233" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G234" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G218" s="5" t="s">
+    <row r="235" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G235" s="4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G219" s="5" t="s">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G236" s="4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G220" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G221" s="5" t="s">
+    <row r="237" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G237" s="4" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G222" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G223" s="5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G224" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G225" s="5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G226" s="5" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G227" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G228" s="5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G229" s="5" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G230" s="5" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G231" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G232" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G233" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G234" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G235" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G236" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G237" s="5" t="s">
-        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2889,21 +3169,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100203199D83812C2499E49CC0C3E7DE06C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2f8823872235ddf1d1c55d8837f3ca9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="631437c1-70b7-41ea-97e4-3973abe7cce0" xmlns:ns4="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="116abd7a6875440f2166ad9e25254cea" ns3:_="" ns4:_="">
     <xsd:import namespace="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
@@ -3112,32 +3377,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F8F7E8B-C071-4DC9-A2E9-BDAF31C19E75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{214CF277-9889-499D-8A02-51B999F78EC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3154,4 +3409,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F8F7E8B-C071-4DC9-A2E9-BDAF31C19E75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(fe-piattaforma): fe updates 10212022
</commit_message>
<xml_diff>
--- a/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
+++ b/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.zappa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna.a.orlando/Desktop/MITD/public/assets/entity_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AA2B79-2828-4DB9-8E58-E32F53D08181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0388A139-B45D-7F47-BE5F-8D2DA952A09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24160" windowHeight="14260" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>Dipendente a tempo determinato</t>
   </si>
   <si>
-    <t>Straniera, di un Paese ALL'INTERNO dell'Unione Europea</t>
-  </si>
-  <si>
     <t>Percettore di sussidio di disabilità</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Diploma di scuola superiore (diploma di maturità) / Scuola secondaria di II grado (5 anni)</t>
   </si>
   <si>
-    <t>Straniera, di un Paese AL DI FUORI dell'Unione Europea</t>
-  </si>
-  <si>
     <t>Altro percettore di sussidio (es.: reddito di cittadinanza)</t>
   </si>
   <si>
@@ -905,6 +899,12 @@
   </si>
   <si>
     <t>BCCMRC53A16T995Y</t>
+  </si>
+  <si>
+    <t>Straniera, di un Paese AL DI FUORI dell’Unione Europea</t>
+  </si>
+  <si>
+    <t>Straniera, di un Paese ALL’INTERNO dell’Unione Europea</t>
   </si>
 </sst>
 </file>
@@ -959,8 +959,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -976,7 +976,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1274,17 +1274,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8BEB98-427E-496B-B7BD-F71A2D02D0A0}">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="12.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="42.1640625" customWidth="1"/>
+    <col min="11" max="16" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1334,15 +1336,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1350,16 +1352,16 @@
         <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>21</v>
@@ -1380,399 +1382,399 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
     </row>
-    <row r="99" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
     </row>
-    <row r="101" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="8:17" x14ac:dyDescent="0.2">
       <c r="Q101">
         <v>0</v>
       </c>
@@ -1841,21 +1843,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA2305A-781D-4ABB-83F9-A2AAD4F5F6E0}">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="22.36328125" customWidth="1"/>
+    <col min="5" max="5" width="39.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1878,7 +1880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1901,7 +1903,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1915,1252 +1917,1252 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
+        <v>289</v>
+      </c>
+      <c r="F3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="C5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
         <v>47</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="D7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
+      <c r="G7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="D8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
+      <c r="G8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
+      <c r="G9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D12" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="4" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="4" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G15" s="4" t="s">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G16" s="4" t="s">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G17" s="4" t="s">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G18" s="4" t="s">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G19" s="4" t="s">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G20" s="4" t="s">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G21" s="1" t="s">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G22" s="4" t="s">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G23" s="4" t="s">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G24" s="4" t="s">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G25" s="4" t="s">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G26" s="4" t="s">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G27" s="4" t="s">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G28" s="4" t="s">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G29" s="4" t="s">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G30" s="4" t="s">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G31" s="4" t="s">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G32" s="4" t="s">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G33" s="4" t="s">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G34" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G35" s="4" t="s">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G36" s="4" t="s">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G37" s="4" t="s">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G40" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G38" s="4" t="s">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G39" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G40" s="4" t="s">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G41" s="4" t="s">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G42" s="4" t="s">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G43" s="4" t="s">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G44" s="4" t="s">
+    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G45" s="4" t="s">
+    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G46" s="4" t="s">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G48" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G47" s="4" t="s">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G49" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G48" s="4" t="s">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G50" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G49" s="4" t="s">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G51" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G50" s="4" t="s">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G52" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G51" s="4" t="s">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G53" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G52" s="4" t="s">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G54" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G53" s="4" t="s">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G55" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G54" s="4" t="s">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G55" s="4" t="s">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G57" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G56" s="4" t="s">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G58" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G57" s="4" t="s">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G59" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G58" s="4" t="s">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G60" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G59" s="4" t="s">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G61" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G60" s="4" t="s">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G62" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G61" s="4" t="s">
+    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G63" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G62" s="4" t="s">
+    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G64" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G63" s="4" t="s">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G65" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G64" s="4" t="s">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G66" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G65" s="4" t="s">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G67" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G66" s="4" t="s">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G68" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G67" s="4" t="s">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G69" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G68" s="4" t="s">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G70" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G69" s="4" t="s">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G71" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G70" s="4" t="s">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G72" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G71" s="4" t="s">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G73" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G72" s="4" t="s">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G74" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G73" s="4" t="s">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G75" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G74" s="4" t="s">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G76" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G75" s="4" t="s">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G77" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G76" s="4" t="s">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G78" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G77" s="4" t="s">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G79" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G78" s="4" t="s">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G80" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G79" s="4" t="s">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G81" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G80" s="4" t="s">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G82" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G81" s="4" t="s">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G83" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G82" s="4" t="s">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G84" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G83" s="4" t="s">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G85" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G84" s="4" t="s">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G86" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G85" s="4" t="s">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G87" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G86" s="4" t="s">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G88" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G87" s="4" t="s">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G89" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G88" s="4" t="s">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G90" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G89" s="4" t="s">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G91" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G90" s="4" t="s">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G92" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G91" s="4" t="s">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G93" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G92" s="4" t="s">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G94" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G93" s="4" t="s">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G95" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G94" s="4" t="s">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G96" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G95" s="4" t="s">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G97" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G96" s="4" t="s">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G98" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G97" s="4" t="s">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G99" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G98" s="4" t="s">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G100" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G99" s="4" t="s">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G101" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G100" s="4" t="s">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G102" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G101" s="4" t="s">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G103" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G102" s="4" t="s">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G104" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G103" s="4" t="s">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G105" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G104" s="4" t="s">
+    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G106" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G105" s="4" t="s">
+    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G107" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G106" s="4" t="s">
+    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G108" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G107" s="4" t="s">
+    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G109" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G108" s="4" t="s">
+    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G110" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G109" s="4" t="s">
+    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G111" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G110" s="4" t="s">
+    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G112" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G111" s="4" t="s">
+    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G113" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G112" s="4" t="s">
+    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G114" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G113" s="4" t="s">
+    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G115" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G114" s="4" t="s">
+    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G116" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G115" s="4" t="s">
+    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G117" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G116" s="4" t="s">
+    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G118" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G117" s="4" t="s">
+    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G119" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G118" s="4" t="s">
+    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G120" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G119" s="4" t="s">
+    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G121" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G120" s="4" t="s">
+    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G122" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G121" s="4" t="s">
+    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G123" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G122" s="4" t="s">
+    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G124" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G123" s="4" t="s">
+    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G125" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G124" s="4" t="s">
+    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G126" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G125" s="4" t="s">
+    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G127" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G126" s="4" t="s">
+    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G128" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G127" s="4" t="s">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G129" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G128" s="4" t="s">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G130" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G131" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G129" s="4" t="s">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G132" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G130" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G131" s="4" t="s">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G133" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G132" s="4" t="s">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G134" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G133" s="4" t="s">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G135" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G134" s="4" t="s">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G136" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G135" s="4" t="s">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G137" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G136" s="4" t="s">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G138" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G137" s="4" t="s">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G139" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G138" s="4" t="s">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G140" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G139" s="4" t="s">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G141" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G140" s="4" t="s">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G142" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G141" s="4" t="s">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G143" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G142" s="4" t="s">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G144" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G143" s="4" t="s">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G145" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G144" s="4" t="s">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G146" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G145" s="4" t="s">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G147" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G146" s="4" t="s">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G148" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G147" s="4" t="s">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G149" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G148" s="4" t="s">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G150" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G149" s="4" t="s">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G151" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G150" s="4" t="s">
+    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G152" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G151" s="4" t="s">
+    <row r="153" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G153" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G152" s="4" t="s">
+    <row r="154" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G154" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="155" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G155" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G153" s="4" t="s">
+    <row r="156" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G156" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G154" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G155" s="4" t="s">
+    <row r="157" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G157" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G156" s="4" t="s">
+    <row r="158" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G158" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G157" s="4" t="s">
+    <row r="159" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G159" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G158" s="4" t="s">
+    <row r="160" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G160" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G159" s="4" t="s">
+    <row r="161" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G161" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G160" s="4" t="s">
+    <row r="162" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G162" s="4" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G161" s="4" t="s">
+    <row r="163" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G163" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G162" s="4" t="s">
+    <row r="164" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G164" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G163" s="4" t="s">
+    <row r="165" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G165" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G164" s="4" t="s">
+    <row r="166" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G166" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G165" s="4" t="s">
+    <row r="167" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G167" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G166" s="4" t="s">
+    <row r="168" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G168" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G167" s="4" t="s">
+    <row r="169" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G169" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G168" s="4" t="s">
+    <row r="170" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G170" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G169" s="4" t="s">
+    <row r="171" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G171" s="4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G170" s="4" t="s">
+    <row r="172" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G172" s="4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G171" s="4" t="s">
+    <row r="173" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G173" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G172" s="4" t="s">
+    <row r="174" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G174" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G173" s="4" t="s">
+    <row r="175" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G175" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G174" s="4" t="s">
+    <row r="176" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G176" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G175" s="4" t="s">
+    <row r="177" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G177" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G176" s="4" t="s">
+    <row r="178" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G178" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G177" s="4" t="s">
+    <row r="179" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G179" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G178" s="4" t="s">
+    <row r="180" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G180" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G179" s="4" t="s">
+    <row r="181" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G181" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G180" s="4" t="s">
+    <row r="182" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G182" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G181" s="4" t="s">
+    <row r="183" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G183" s="4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G182" s="4" t="s">
+    <row r="184" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G184" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G183" s="4" t="s">
+    <row r="185" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G185" s="4" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G184" s="4" t="s">
+    <row r="186" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G186" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G185" s="4" t="s">
+    <row r="187" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G187" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G186" s="4" t="s">
+    <row r="188" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G188" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G187" s="4" t="s">
+    <row r="189" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G189" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G188" s="4" t="s">
+    <row r="190" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G190" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G189" s="4" t="s">
+    <row r="191" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G191" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G190" s="4" t="s">
+    <row r="192" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G192" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G191" s="4" t="s">
+    <row r="193" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G193" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G192" s="4" t="s">
+    <row r="194" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G194" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G193" s="4" t="s">
+    <row r="195" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G195" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G194" s="4" t="s">
+    <row r="196" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G196" s="4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G195" s="4" t="s">
+    <row r="197" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G197" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G196" s="4" t="s">
+    <row r="198" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G198" s="4" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G197" s="4" t="s">
+    <row r="199" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G199" s="4" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G198" s="4" t="s">
+    <row r="200" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G200" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G199" s="4" t="s">
+    <row r="201" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G201" s="4" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G200" s="4" t="s">
+    <row r="202" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G202" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G201" s="4" t="s">
+    <row r="203" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G203" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G202" s="4" t="s">
+    <row r="204" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G204" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G203" s="4" t="s">
+    <row r="205" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G205" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G204" s="4" t="s">
+    <row r="206" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G206" s="4" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G205" s="4" t="s">
+    <row r="207" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G207" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G206" s="4" t="s">
+    <row r="208" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G208" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G207" s="4" t="s">
+    <row r="209" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G209" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G208" s="4" t="s">
+    <row r="210" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G210" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G209" s="4" t="s">
+    <row r="211" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G211" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G210" s="4" t="s">
+    <row r="212" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G212" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G211" s="4" t="s">
+    <row r="213" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G213" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G212" s="4" t="s">
+    <row r="214" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G214" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G213" s="4" t="s">
+    <row r="215" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G215" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G214" s="4" t="s">
+    <row r="216" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G216" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G215" s="4" t="s">
+    <row r="217" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G217" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G216" s="4" t="s">
+    <row r="218" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G218" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G217" s="4" t="s">
+    <row r="219" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G219" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G218" s="4" t="s">
+    <row r="220" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G220" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="221" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G221" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G219" s="4" t="s">
+    <row r="222" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G222" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G220" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G221" s="4" t="s">
+    <row r="223" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G223" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G222" s="4" t="s">
+    <row r="224" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G224" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G223" s="4" t="s">
+    <row r="225" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G225" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G224" s="4" t="s">
+    <row r="226" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G226" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G225" s="4" t="s">
+    <row r="227" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G227" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G226" s="4" t="s">
+    <row r="228" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G228" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G227" s="4" t="s">
+    <row r="229" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G229" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G228" s="4" t="s">
+    <row r="230" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G230" s="4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G229" s="4" t="s">
+    <row r="231" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G231" s="4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G230" s="4" t="s">
+    <row r="232" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G232" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G231" s="4" t="s">
+    <row r="233" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G233" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G234" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G232" s="4" t="s">
+    <row r="235" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G235" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G233" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G234" s="4" t="s">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G236" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G235" s="4" t="s">
+    <row r="237" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G237" s="4" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G236" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G237" s="4" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3378,18 +3380,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3412,14 +3414,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F8F7E8B-C071-4DC9-A2E9-BDAF31C19E75}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3434,4 +3428,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(fe-piattaforma): fe updates 10242022
</commit_message>
<xml_diff>
--- a/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
+++ b/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.zappa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna.a.orlando/Desktop/MITD/public/assets/entity_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AA2B79-2828-4DB9-8E58-E32F53D08181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0388A139-B45D-7F47-BE5F-8D2DA952A09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24160" windowHeight="14260" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>Dipendente a tempo determinato</t>
   </si>
   <si>
-    <t>Straniera, di un Paese ALL'INTERNO dell'Unione Europea</t>
-  </si>
-  <si>
     <t>Percettore di sussidio di disabilità</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Diploma di scuola superiore (diploma di maturità) / Scuola secondaria di II grado (5 anni)</t>
   </si>
   <si>
-    <t>Straniera, di un Paese AL DI FUORI dell'Unione Europea</t>
-  </si>
-  <si>
     <t>Altro percettore di sussidio (es.: reddito di cittadinanza)</t>
   </si>
   <si>
@@ -905,6 +899,12 @@
   </si>
   <si>
     <t>BCCMRC53A16T995Y</t>
+  </si>
+  <si>
+    <t>Straniera, di un Paese AL DI FUORI dell’Unione Europea</t>
+  </si>
+  <si>
+    <t>Straniera, di un Paese ALL’INTERNO dell’Unione Europea</t>
   </si>
 </sst>
 </file>
@@ -959,8 +959,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -976,7 +976,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1274,17 +1274,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8BEB98-427E-496B-B7BD-F71A2D02D0A0}">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="12.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="42.1640625" customWidth="1"/>
+    <col min="11" max="16" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1334,15 +1336,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1350,16 +1352,16 @@
         <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>21</v>
@@ -1380,399 +1382,399 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
     </row>
-    <row r="99" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
     </row>
-    <row r="101" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="8:17" x14ac:dyDescent="0.2">
       <c r="Q101">
         <v>0</v>
       </c>
@@ -1841,21 +1843,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA2305A-781D-4ABB-83F9-A2AAD4F5F6E0}">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="22.36328125" customWidth="1"/>
+    <col min="5" max="5" width="39.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1878,7 +1880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1901,7 +1903,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1915,1252 +1917,1252 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
+        <v>289</v>
+      </c>
+      <c r="F3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="C5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
         <v>47</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="D7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
+      <c r="G7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="D8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
+      <c r="G8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
+      <c r="G9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D12" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="4" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="4" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G15" s="4" t="s">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G16" s="4" t="s">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G17" s="4" t="s">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G18" s="4" t="s">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G19" s="4" t="s">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G20" s="4" t="s">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G21" s="1" t="s">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G22" s="4" t="s">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G23" s="4" t="s">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G24" s="4" t="s">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G25" s="4" t="s">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G26" s="4" t="s">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G27" s="4" t="s">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G28" s="4" t="s">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G29" s="4" t="s">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G30" s="4" t="s">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G31" s="4" t="s">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G32" s="4" t="s">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G33" s="4" t="s">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G34" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G35" s="4" t="s">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G36" s="4" t="s">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G37" s="4" t="s">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G40" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G38" s="4" t="s">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G39" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G40" s="4" t="s">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G41" s="4" t="s">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G42" s="4" t="s">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G43" s="4" t="s">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G44" s="4" t="s">
+    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G45" s="4" t="s">
+    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G46" s="4" t="s">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G48" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G47" s="4" t="s">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G49" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G48" s="4" t="s">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G50" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G49" s="4" t="s">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G51" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G50" s="4" t="s">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G52" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G51" s="4" t="s">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G53" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G52" s="4" t="s">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G54" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G53" s="4" t="s">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G55" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G54" s="4" t="s">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G55" s="4" t="s">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G57" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G56" s="4" t="s">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G58" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G57" s="4" t="s">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G59" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G58" s="4" t="s">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G60" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G59" s="4" t="s">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G61" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G60" s="4" t="s">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G62" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G61" s="4" t="s">
+    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G63" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G62" s="4" t="s">
+    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G64" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G63" s="4" t="s">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G65" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G64" s="4" t="s">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G66" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G65" s="4" t="s">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G67" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G66" s="4" t="s">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G68" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G67" s="4" t="s">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G69" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G68" s="4" t="s">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G70" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G69" s="4" t="s">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G71" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G70" s="4" t="s">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G72" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G71" s="4" t="s">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G73" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G72" s="4" t="s">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G74" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G73" s="4" t="s">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G75" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G74" s="4" t="s">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G76" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G75" s="4" t="s">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G77" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G76" s="4" t="s">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G78" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G77" s="4" t="s">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G79" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G78" s="4" t="s">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G80" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G79" s="4" t="s">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G81" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G80" s="4" t="s">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G82" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G81" s="4" t="s">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G83" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G82" s="4" t="s">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G84" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G83" s="4" t="s">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G85" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G84" s="4" t="s">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G86" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G85" s="4" t="s">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G87" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G86" s="4" t="s">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G88" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G87" s="4" t="s">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G89" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G88" s="4" t="s">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G90" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G89" s="4" t="s">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G91" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G90" s="4" t="s">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G92" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G91" s="4" t="s">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G93" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G92" s="4" t="s">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G94" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G93" s="4" t="s">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G95" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G94" s="4" t="s">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G96" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G95" s="4" t="s">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G97" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G96" s="4" t="s">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G98" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G97" s="4" t="s">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G99" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G98" s="4" t="s">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G100" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G99" s="4" t="s">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G101" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G100" s="4" t="s">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G102" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G101" s="4" t="s">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G103" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G102" s="4" t="s">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G104" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G103" s="4" t="s">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G105" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G104" s="4" t="s">
+    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G106" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G105" s="4" t="s">
+    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G107" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G106" s="4" t="s">
+    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G108" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G107" s="4" t="s">
+    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G109" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G108" s="4" t="s">
+    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G110" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G109" s="4" t="s">
+    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G111" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G110" s="4" t="s">
+    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G112" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G111" s="4" t="s">
+    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G113" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G112" s="4" t="s">
+    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G114" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G113" s="4" t="s">
+    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G115" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G114" s="4" t="s">
+    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G116" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G115" s="4" t="s">
+    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G117" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G116" s="4" t="s">
+    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G118" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G117" s="4" t="s">
+    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G119" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G118" s="4" t="s">
+    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G120" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G119" s="4" t="s">
+    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G121" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G120" s="4" t="s">
+    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G122" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G121" s="4" t="s">
+    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G123" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G122" s="4" t="s">
+    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G124" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G123" s="4" t="s">
+    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G125" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G124" s="4" t="s">
+    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G126" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G125" s="4" t="s">
+    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G127" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G126" s="4" t="s">
+    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G128" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G127" s="4" t="s">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G129" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G128" s="4" t="s">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G130" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G131" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G129" s="4" t="s">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G132" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G130" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G131" s="4" t="s">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G133" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G132" s="4" t="s">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G134" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G133" s="4" t="s">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G135" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G134" s="4" t="s">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G136" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G135" s="4" t="s">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G137" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G136" s="4" t="s">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G138" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G137" s="4" t="s">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G139" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G138" s="4" t="s">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G140" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G139" s="4" t="s">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G141" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G140" s="4" t="s">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G142" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G141" s="4" t="s">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G143" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G142" s="4" t="s">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G144" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G143" s="4" t="s">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G145" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G144" s="4" t="s">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G146" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G145" s="4" t="s">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G147" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G146" s="4" t="s">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G148" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G147" s="4" t="s">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G149" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G148" s="4" t="s">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G150" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G149" s="4" t="s">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G151" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G150" s="4" t="s">
+    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G152" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G151" s="4" t="s">
+    <row r="153" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G153" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G152" s="4" t="s">
+    <row r="154" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G154" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="155" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G155" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G153" s="4" t="s">
+    <row r="156" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G156" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G154" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G155" s="4" t="s">
+    <row r="157" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G157" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G156" s="4" t="s">
+    <row r="158" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G158" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G157" s="4" t="s">
+    <row r="159" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G159" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G158" s="4" t="s">
+    <row r="160" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G160" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G159" s="4" t="s">
+    <row r="161" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G161" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G160" s="4" t="s">
+    <row r="162" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G162" s="4" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G161" s="4" t="s">
+    <row r="163" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G163" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G162" s="4" t="s">
+    <row r="164" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G164" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G163" s="4" t="s">
+    <row r="165" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G165" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G164" s="4" t="s">
+    <row r="166" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G166" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G165" s="4" t="s">
+    <row r="167" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G167" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G166" s="4" t="s">
+    <row r="168" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G168" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G167" s="4" t="s">
+    <row r="169" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G169" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G168" s="4" t="s">
+    <row r="170" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G170" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G169" s="4" t="s">
+    <row r="171" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G171" s="4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G170" s="4" t="s">
+    <row r="172" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G172" s="4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G171" s="4" t="s">
+    <row r="173" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G173" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G172" s="4" t="s">
+    <row r="174" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G174" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G173" s="4" t="s">
+    <row r="175" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G175" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G174" s="4" t="s">
+    <row r="176" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G176" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G175" s="4" t="s">
+    <row r="177" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G177" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G176" s="4" t="s">
+    <row r="178" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G178" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G177" s="4" t="s">
+    <row r="179" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G179" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G178" s="4" t="s">
+    <row r="180" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G180" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G179" s="4" t="s">
+    <row r="181" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G181" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G180" s="4" t="s">
+    <row r="182" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G182" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G181" s="4" t="s">
+    <row r="183" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G183" s="4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G182" s="4" t="s">
+    <row r="184" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G184" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G183" s="4" t="s">
+    <row r="185" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G185" s="4" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G184" s="4" t="s">
+    <row r="186" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G186" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G185" s="4" t="s">
+    <row r="187" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G187" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G186" s="4" t="s">
+    <row r="188" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G188" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G187" s="4" t="s">
+    <row r="189" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G189" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G188" s="4" t="s">
+    <row r="190" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G190" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G189" s="4" t="s">
+    <row r="191" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G191" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G190" s="4" t="s">
+    <row r="192" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G192" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G191" s="4" t="s">
+    <row r="193" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G193" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G192" s="4" t="s">
+    <row r="194" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G194" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G193" s="4" t="s">
+    <row r="195" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G195" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G194" s="4" t="s">
+    <row r="196" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G196" s="4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G195" s="4" t="s">
+    <row r="197" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G197" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G196" s="4" t="s">
+    <row r="198" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G198" s="4" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G197" s="4" t="s">
+    <row r="199" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G199" s="4" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G198" s="4" t="s">
+    <row r="200" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G200" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G199" s="4" t="s">
+    <row r="201" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G201" s="4" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G200" s="4" t="s">
+    <row r="202" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G202" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G201" s="4" t="s">
+    <row r="203" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G203" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G202" s="4" t="s">
+    <row r="204" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G204" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G203" s="4" t="s">
+    <row r="205" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G205" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G204" s="4" t="s">
+    <row r="206" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G206" s="4" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G205" s="4" t="s">
+    <row r="207" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G207" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G206" s="4" t="s">
+    <row r="208" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G208" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G207" s="4" t="s">
+    <row r="209" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G209" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G208" s="4" t="s">
+    <row r="210" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G210" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G209" s="4" t="s">
+    <row r="211" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G211" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G210" s="4" t="s">
+    <row r="212" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G212" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G211" s="4" t="s">
+    <row r="213" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G213" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G212" s="4" t="s">
+    <row r="214" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G214" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G213" s="4" t="s">
+    <row r="215" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G215" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G214" s="4" t="s">
+    <row r="216" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G216" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G215" s="4" t="s">
+    <row r="217" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G217" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G216" s="4" t="s">
+    <row r="218" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G218" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G217" s="4" t="s">
+    <row r="219" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G219" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G218" s="4" t="s">
+    <row r="220" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G220" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="221" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G221" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G219" s="4" t="s">
+    <row r="222" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G222" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G220" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G221" s="4" t="s">
+    <row r="223" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G223" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G222" s="4" t="s">
+    <row r="224" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G224" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G223" s="4" t="s">
+    <row r="225" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G225" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G224" s="4" t="s">
+    <row r="226" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G226" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G225" s="4" t="s">
+    <row r="227" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G227" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G226" s="4" t="s">
+    <row r="228" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G228" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G227" s="4" t="s">
+    <row r="229" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G229" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G228" s="4" t="s">
+    <row r="230" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G230" s="4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G229" s="4" t="s">
+    <row r="231" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G231" s="4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G230" s="4" t="s">
+    <row r="232" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G232" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G231" s="4" t="s">
+    <row r="233" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G233" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G234" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G232" s="4" t="s">
+    <row r="235" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G235" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G233" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G234" s="4" t="s">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G236" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G235" s="4" t="s">
+    <row r="237" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G237" s="4" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G236" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G237" s="4" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3378,18 +3380,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3412,14 +3414,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F8F7E8B-C071-4DC9-A2E9-BDAF31C19E75}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3434,4 +3428,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(fe-piattaforma): fe updates 10252022
</commit_message>
<xml_diff>
--- a/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
+++ b/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna.a.orlando/Desktop/MITD/public/assets/entity_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0388A139-B45D-7F47-BE5F-8D2DA952A09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57587E77-665C-444A-BC03-39957B1A3E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24160" windowHeight="14260" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="282">
   <si>
     <t>CodiceFiscale</t>
   </si>
@@ -100,24 +100,12 @@
     <t>Italiana</t>
   </si>
   <si>
-    <t>MILANO</t>
-  </si>
-  <si>
     <t>Rifugiato/ Migrante</t>
   </si>
   <si>
-    <t>piattaforma_facilitazione@yopmail.com</t>
-  </si>
-  <si>
     <t>+39</t>
   </si>
   <si>
-    <t>3332323111</t>
-  </si>
-  <si>
-    <t>02561616</t>
-  </si>
-  <si>
     <t>Titolo di studio</t>
   </si>
   <si>
@@ -887,18 +875,6 @@
   </si>
   <si>
     <t>+263</t>
-  </si>
-  <si>
-    <t>1953</t>
-  </si>
-  <si>
-    <t>MARCO</t>
-  </si>
-  <si>
-    <t>BICCI</t>
-  </si>
-  <si>
-    <t>BCCMRC53A16T995Y</t>
   </si>
   <si>
     <t>Straniera, di un Paese AL DI FUORI dell’Unione Europea</t>
@@ -911,18 +887,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -945,21 +913,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1272,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8BEB98-427E-496B-B7BD-F71A2D02D0A0}">
-  <dimension ref="A1:Q101"/>
+  <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1336,51 +1301,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>26</v>
-      </c>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H3" s="1"/>
@@ -1771,23 +1694,13 @@
       <c r="I99" s="1"/>
     </row>
     <row r="100" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-    </row>
-    <row r="101" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="Q101">
+      <c r="Q100">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{F351616E-F65B-4FE8-A381-7F8849054211}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <ignoredErrors>
-    <ignoredError sqref="G2" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
@@ -1795,43 +1708,43 @@
           <x14:formula1>
             <xm:f>valori!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L101</xm:sqref>
+          <xm:sqref>L2:L100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C0FA6E0-F7E0-4DC8-B25F-A72B4D311A58}">
           <x14:formula1>
             <xm:f>valori!$C$2:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H100</xm:sqref>
+          <xm:sqref>H2:H99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AE43BD5-0167-4321-B099-FDE2FB6A1933}">
           <x14:formula1>
             <xm:f>valori!$D$2:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I100</xm:sqref>
+          <xm:sqref>I2:I99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{982C8DCC-435C-421D-8EA1-21A053C25223}">
           <x14:formula1>
             <xm:f>valori!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J100</xm:sqref>
+          <xm:sqref>J2:J99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECD8C6CC-EDBD-48A8-A51C-9053D522AE1F}">
           <x14:formula1>
             <xm:f>valori!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D100</xm:sqref>
+          <xm:sqref>D2:D99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCF0EE29-51E8-4E2A-B6CD-216BA845A309}">
           <x14:formula1>
             <xm:f>valori!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F101</xm:sqref>
+          <xm:sqref>F2:F100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50897BB4-255D-43E6-8928-804484AA2B28}">
           <x14:formula1>
             <xm:f>valori!$G$2:$G$237</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N101</xm:sqref>
+          <xm:sqref>N2:N100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1865,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1874,7 +1787,7 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
@@ -1885,27 +1798,27 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1914,1255 +1827,1255 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G15" s="4" t="s">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G16" s="4" t="s">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="3" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G18" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G19" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G20" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G22" s="4" t="s">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G23" s="4" t="s">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G24" s="4" t="s">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G25" s="4" t="s">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G26" s="4" t="s">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G27" s="4" t="s">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G28" s="4" t="s">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G29" s="4" t="s">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G30" s="4" t="s">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G31" s="4" t="s">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G32" s="4" t="s">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G33" s="4" t="s">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G34" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G35" s="4" t="s">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G40" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G36" s="4" t="s">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G37" s="4" t="s">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G38" s="4" t="s">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G39" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G40" s="4" t="s">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G41" s="4" t="s">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G42" s="4" t="s">
+    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="4" t="s">
+    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G44" s="4" t="s">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G48" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G45" s="4" t="s">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G49" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G46" s="4" t="s">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G50" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G47" s="4" t="s">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G51" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G48" s="4" t="s">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G52" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G49" s="4" t="s">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G53" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G50" s="4" t="s">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G54" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G51" s="4" t="s">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G55" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G52" s="4" t="s">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G53" s="4" t="s">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G57" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G54" s="4" t="s">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G58" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G55" s="4" t="s">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G59" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G56" s="4" t="s">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G60" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G57" s="4" t="s">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G61" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G58" s="4" t="s">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G62" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G59" s="4" t="s">
+    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G63" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G60" s="4" t="s">
+    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G64" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G61" s="4" t="s">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G65" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G62" s="4" t="s">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G66" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G63" s="4" t="s">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G67" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G64" s="4" t="s">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G68" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G65" s="4" t="s">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G69" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G66" s="4" t="s">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G70" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G67" s="4" t="s">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G71" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G68" s="4" t="s">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G72" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G69" s="4" t="s">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G73" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G70" s="4" t="s">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G74" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G71" s="4" t="s">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G75" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G72" s="4" t="s">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G76" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G73" s="4" t="s">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G77" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G74" s="4" t="s">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G78" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G75" s="4" t="s">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G79" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G76" s="4" t="s">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G80" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G77" s="4" t="s">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G81" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G78" s="4" t="s">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G82" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G79" s="4" t="s">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G83" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G80" s="4" t="s">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G84" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G81" s="4" t="s">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G85" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G82" s="4" t="s">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G86" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G83" s="4" t="s">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G87" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G84" s="4" t="s">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G88" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G85" s="4" t="s">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G89" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G86" s="4" t="s">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G90" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G87" s="4" t="s">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G91" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G88" s="4" t="s">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G92" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G89" s="4" t="s">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G93" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G90" s="4" t="s">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G94" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G91" s="4" t="s">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G95" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G92" s="4" t="s">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G96" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G93" s="4" t="s">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G97" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G94" s="4" t="s">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G98" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G95" s="4" t="s">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G99" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G96" s="4" t="s">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G100" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G97" s="4" t="s">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G101" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G98" s="4" t="s">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G102" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G99" s="4" t="s">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G103" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G100" s="4" t="s">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G104" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G101" s="4" t="s">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G105" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G102" s="4" t="s">
+    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G106" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G103" s="4" t="s">
+    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G107" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G104" s="4" t="s">
+    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G108" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G105" s="4" t="s">
+    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G109" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G106" s="4" t="s">
+    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G110" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G107" s="4" t="s">
+    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G111" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G108" s="4" t="s">
+    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G112" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G109" s="4" t="s">
+    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G113" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G110" s="4" t="s">
+    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G114" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G111" s="4" t="s">
+    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G115" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G112" s="4" t="s">
+    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G116" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G113" s="4" t="s">
+    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G117" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G114" s="4" t="s">
+    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G118" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G115" s="4" t="s">
+    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G119" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G116" s="4" t="s">
+    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G120" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G117" s="4" t="s">
+    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G121" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G118" s="4" t="s">
+    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G122" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G119" s="4" t="s">
+    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G123" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G120" s="4" t="s">
+    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G124" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G121" s="4" t="s">
+    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G125" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G122" s="4" t="s">
+    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G126" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G123" s="4" t="s">
+    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G127" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G124" s="4" t="s">
+    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G128" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G125" s="4" t="s">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G129" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G126" s="4" t="s">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G130" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G131" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G127" s="4" t="s">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G132" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G128" s="4" t="s">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G133" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G129" s="4" t="s">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G134" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G130" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G131" s="4" t="s">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G135" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G132" s="4" t="s">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G136" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G133" s="4" t="s">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G137" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G134" s="4" t="s">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G138" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G135" s="4" t="s">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G139" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G136" s="4" t="s">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G140" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G137" s="4" t="s">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G141" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G138" s="4" t="s">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G142" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G139" s="4" t="s">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G143" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G140" s="4" t="s">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G144" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G141" s="4" t="s">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G145" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G142" s="4" t="s">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G146" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G143" s="4" t="s">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G147" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G144" s="4" t="s">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G148" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G145" s="4" t="s">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G149" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G146" s="4" t="s">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G150" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G147" s="4" t="s">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G151" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G148" s="4" t="s">
+    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G152" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G149" s="4" t="s">
+    <row r="153" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G153" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G150" s="4" t="s">
+    <row r="154" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G154" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="155" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G155" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G151" s="4" t="s">
+    <row r="156" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G156" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G152" s="4" t="s">
+    <row r="157" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G157" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G153" s="4" t="s">
+    <row r="158" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G158" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G154" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G155" s="4" t="s">
+    <row r="159" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G159" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G156" s="4" t="s">
+    <row r="160" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G160" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G157" s="4" t="s">
+    <row r="161" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G161" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G158" s="4" t="s">
+    <row r="162" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G162" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G159" s="4" t="s">
+    <row r="163" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G163" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G160" s="4" t="s">
+    <row r="164" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G164" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G161" s="4" t="s">
+    <row r="165" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G165" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G162" s="4" t="s">
+    <row r="166" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G166" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G163" s="4" t="s">
+    <row r="167" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G167" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G164" s="4" t="s">
+    <row r="168" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G168" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G165" s="4" t="s">
+    <row r="169" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G169" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G166" s="4" t="s">
+    <row r="170" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G170" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G167" s="4" t="s">
+    <row r="171" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G171" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G168" s="4" t="s">
+    <row r="172" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G172" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G169" s="4" t="s">
+    <row r="173" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G173" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G170" s="4" t="s">
+    <row r="174" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G174" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G171" s="4" t="s">
+    <row r="175" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G175" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G172" s="4" t="s">
+    <row r="176" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G176" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G173" s="4" t="s">
+    <row r="177" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G177" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G174" s="4" t="s">
+    <row r="178" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G178" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G175" s="4" t="s">
+    <row r="179" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G179" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G176" s="4" t="s">
+    <row r="180" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G180" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G177" s="4" t="s">
+    <row r="181" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G181" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G178" s="4" t="s">
+    <row r="182" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G182" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G179" s="4" t="s">
+    <row r="183" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G183" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G180" s="4" t="s">
+    <row r="184" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G184" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G181" s="4" t="s">
+    <row r="185" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G185" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G182" s="4" t="s">
+    <row r="186" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G186" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G183" s="4" t="s">
+    <row r="187" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G187" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G184" s="4" t="s">
+    <row r="188" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G188" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G185" s="4" t="s">
+    <row r="189" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G189" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G186" s="4" t="s">
+    <row r="190" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G190" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G187" s="4" t="s">
+    <row r="191" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G191" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G188" s="4" t="s">
+    <row r="192" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G192" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G189" s="4" t="s">
+    <row r="193" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G193" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G190" s="4" t="s">
+    <row r="194" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G194" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G191" s="4" t="s">
+    <row r="195" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G195" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G192" s="4" t="s">
+    <row r="196" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G196" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G193" s="4" t="s">
+    <row r="197" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G197" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G194" s="4" t="s">
+    <row r="198" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G198" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G195" s="4" t="s">
+    <row r="199" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G199" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G196" s="4" t="s">
+    <row r="200" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G200" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G197" s="4" t="s">
+    <row r="201" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G201" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G198" s="4" t="s">
+    <row r="202" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G202" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G199" s="4" t="s">
+    <row r="203" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G203" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G200" s="4" t="s">
+    <row r="204" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G204" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G201" s="4" t="s">
+    <row r="205" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G205" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G202" s="4" t="s">
+    <row r="206" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G206" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G203" s="4" t="s">
+    <row r="207" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G207" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G204" s="4" t="s">
+    <row r="208" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G208" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G205" s="4" t="s">
+    <row r="209" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G209" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G206" s="4" t="s">
+    <row r="210" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G210" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G207" s="4" t="s">
+    <row r="211" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G211" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G208" s="4" t="s">
+    <row r="212" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G212" s="3" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G209" s="4" t="s">
+    <row r="213" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G213" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G210" s="4" t="s">
+    <row r="214" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G214" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G211" s="4" t="s">
+    <row r="215" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G215" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G212" s="4" t="s">
+    <row r="216" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G216" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G213" s="4" t="s">
+    <row r="217" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G217" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G214" s="4" t="s">
+    <row r="218" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G218" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G215" s="4" t="s">
+    <row r="219" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G219" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G216" s="4" t="s">
+    <row r="220" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G220" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="221" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G221" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G217" s="4" t="s">
+    <row r="222" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G222" s="3" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G218" s="4" t="s">
+    <row r="223" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G223" s="3" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G219" s="4" t="s">
+    <row r="224" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G224" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G220" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G221" s="4" t="s">
+    <row r="225" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G225" s="3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G222" s="4" t="s">
+    <row r="226" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G226" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G223" s="4" t="s">
+    <row r="227" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G227" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G224" s="4" t="s">
+    <row r="228" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G228" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G225" s="4" t="s">
+    <row r="229" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G229" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G226" s="4" t="s">
+    <row r="230" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G230" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G227" s="4" t="s">
+    <row r="231" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G231" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G228" s="4" t="s">
+    <row r="232" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G232" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G229" s="4" t="s">
+    <row r="233" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G233" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G234" s="3" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G230" s="4" t="s">
+    <row r="235" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G235" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G231" s="4" t="s">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G236" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G232" s="4" t="s">
+    <row r="237" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G237" s="3" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G233" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G234" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G235" s="4" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G236" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G237" s="4" t="s">
-        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3171,6 +3084,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100203199D83812C2499E49CC0C3E7DE06C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2f8823872235ddf1d1c55d8837f3ca9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="631437c1-70b7-41ea-97e4-3973abe7cce0" xmlns:ns4="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="116abd7a6875440f2166ad9e25254cea" ns3:_="" ns4:_="">
     <xsd:import namespace="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
@@ -3379,12 +3298,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3395,6 +3308,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F8F7E8B-C071-4DC9-A2E9-BDAF31C19E75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{214CF277-9889-499D-8A02-51B999F78EC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3413,23 +3343,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F8F7E8B-C071-4DC9-A2E9-BDAF31C19E75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat(fe-piattaforma): fe updates 10262022
</commit_message>
<xml_diff>
--- a/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
+++ b/fe-piattaforma/public/assets/entity_templates/template_cittadino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.zappa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna.a.orlando/Desktop/MITD/public/assets/entity_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AA2B79-2828-4DB9-8E58-E32F53D08181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57587E77-665C-444A-BC03-39957B1A3E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24160" windowHeight="14260" xr2:uid="{151C91AA-01A3-4D16-B1DE-65709FE5A433}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="282">
   <si>
     <t>CodiceFiscale</t>
   </si>
@@ -100,24 +100,12 @@
     <t>Italiana</t>
   </si>
   <si>
-    <t>MILANO</t>
-  </si>
-  <si>
     <t>Rifugiato/ Migrante</t>
   </si>
   <si>
-    <t>piattaforma_facilitazione@yopmail.com</t>
-  </si>
-  <si>
     <t>+39</t>
   </si>
   <si>
-    <t>3332323111</t>
-  </si>
-  <si>
-    <t>02561616</t>
-  </si>
-  <si>
     <t>Titolo di studio</t>
   </si>
   <si>
@@ -139,9 +127,6 @@
     <t>Dipendente a tempo determinato</t>
   </si>
   <si>
-    <t>Straniera, di un Paese ALL'INTERNO dell'Unione Europea</t>
-  </si>
-  <si>
     <t>Percettore di sussidio di disabilità</t>
   </si>
   <si>
@@ -157,9 +142,6 @@
     <t>Diploma di scuola superiore (diploma di maturità) / Scuola secondaria di II grado (5 anni)</t>
   </si>
   <si>
-    <t>Straniera, di un Paese AL DI FUORI dell'Unione Europea</t>
-  </si>
-  <si>
     <t>Altro percettore di sussidio (es.: reddito di cittadinanza)</t>
   </si>
   <si>
@@ -895,34 +877,20 @@
     <t>+263</t>
   </si>
   <si>
-    <t>1953</t>
-  </si>
-  <si>
-    <t>MARCO</t>
-  </si>
-  <si>
-    <t>BICCI</t>
-  </si>
-  <si>
-    <t>BCCMRC53A16T995Y</t>
+    <t>Straniera, di un Paese AL DI FUORI dell’Unione Europea</t>
+  </si>
+  <si>
+    <t>Straniera, di un Paese ALL’INTERNO dell’Unione Europea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -945,22 +913,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -976,7 +941,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1272,19 +1237,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8BEB98-427E-496B-B7BD-F71A2D02D0A0}">
-  <dimension ref="A1:Q101"/>
+  <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="12.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="42.1640625" customWidth="1"/>
+    <col min="11" max="16" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1334,458 +1301,406 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
     </row>
-    <row r="99" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="8:17" x14ac:dyDescent="0.35">
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-    </row>
-    <row r="101" spans="8:17" x14ac:dyDescent="0.35">
-      <c r="Q101">
+    <row r="100" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="Q100">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{F351616E-F65B-4FE8-A381-7F8849054211}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <ignoredErrors>
-    <ignoredError sqref="G2" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
@@ -1793,43 +1708,43 @@
           <x14:formula1>
             <xm:f>valori!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L101</xm:sqref>
+          <xm:sqref>L2:L100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C0FA6E0-F7E0-4DC8-B25F-A72B4D311A58}">
           <x14:formula1>
             <xm:f>valori!$C$2:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H100</xm:sqref>
+          <xm:sqref>H2:H99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AE43BD5-0167-4321-B099-FDE2FB6A1933}">
           <x14:formula1>
             <xm:f>valori!$D$2:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I100</xm:sqref>
+          <xm:sqref>I2:I99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{982C8DCC-435C-421D-8EA1-21A053C25223}">
           <x14:formula1>
             <xm:f>valori!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J100</xm:sqref>
+          <xm:sqref>J2:J99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECD8C6CC-EDBD-48A8-A51C-9053D522AE1F}">
           <x14:formula1>
             <xm:f>valori!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D100</xm:sqref>
+          <xm:sqref>D2:D99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCF0EE29-51E8-4E2A-B6CD-216BA845A309}">
           <x14:formula1>
             <xm:f>valori!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F101</xm:sqref>
+          <xm:sqref>F2:F100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50897BB4-255D-43E6-8928-804484AA2B28}">
           <x14:formula1>
             <xm:f>valori!$G$2:$G$237</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N101</xm:sqref>
+          <xm:sqref>N2:N100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1841,21 +1756,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA2305A-781D-4ABB-83F9-A2AAD4F5F6E0}">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="22.36328125" customWidth="1"/>
+    <col min="5" max="5" width="39.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1863,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1872,38 +1787,38 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1912,1255 +1827,1255 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
         <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
+        <v>280</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="D7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="G7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>48</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>51</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
         <v>54</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="4" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
+      <c r="G11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D10" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="4" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D12" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="4" t="s">
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D13" t="s">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="4" t="s">
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="4" t="s">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G15" s="4" t="s">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G16" s="4" t="s">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G17" s="4" t="s">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G18" s="4" t="s">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G19" s="4" t="s">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G20" s="4" t="s">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G21" s="1" t="s">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G22" s="4" t="s">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G23" s="4" t="s">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G24" s="4" t="s">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G25" s="4" t="s">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G26" s="4" t="s">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G27" s="4" t="s">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G28" s="4" t="s">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G29" s="4" t="s">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G30" s="4" t="s">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G31" s="4" t="s">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G32" s="4" t="s">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G40" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G33" s="4" t="s">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G34" s="4" t="s">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G48" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G49" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G50" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G51" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G52" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G53" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G54" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G55" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G57" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G58" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G59" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G60" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G61" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G62" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G63" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G64" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G65" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G66" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G67" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G68" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G69" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G70" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G71" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G72" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G73" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G74" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G75" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G76" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G77" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G78" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G79" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G80" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G81" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G82" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G83" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G84" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G85" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G86" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G87" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G88" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G89" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G90" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G91" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G92" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G93" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G94" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G95" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G96" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G97" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G98" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G99" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G100" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G101" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G102" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G103" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G104" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G105" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G106" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G107" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G108" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G109" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G110" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G111" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G112" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G113" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G114" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G115" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G116" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G117" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G118" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G119" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G120" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G121" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G122" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G123" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G124" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G125" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G126" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G127" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G128" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G129" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G130" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G131" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G132" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G133" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G134" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G135" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G136" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G137" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G138" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G139" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G140" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G141" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G142" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G143" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G144" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G145" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G146" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G147" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G148" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G149" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G150" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G151" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G152" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="153" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G153" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="154" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G154" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="155" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G155" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="156" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G156" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="157" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G157" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="158" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G158" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="159" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G159" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="160" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G160" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="161" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G161" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="162" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G162" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="163" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G163" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="164" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G164" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="165" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G165" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="166" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G166" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="167" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G167" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="168" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G168" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="169" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G169" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="170" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G170" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="171" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G171" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="172" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G172" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="173" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G173" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="174" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G174" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="175" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G175" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="176" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G176" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="177" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G177" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="178" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G178" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="179" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G179" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="180" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G180" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="181" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G181" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="182" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G182" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="183" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G183" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="184" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G184" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="185" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G185" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="186" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G186" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="187" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G187" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="188" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G188" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="189" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G189" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="190" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G190" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="191" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G191" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="192" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G192" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="193" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G193" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="194" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G194" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="195" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G195" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="196" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G196" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="197" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G197" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="198" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G198" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="199" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G199" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="200" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G200" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="201" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G201" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="202" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G202" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="203" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G203" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="204" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G204" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="205" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G205" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="206" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G206" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="207" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G207" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="208" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G208" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="209" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G209" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="210" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G210" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="211" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G211" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="212" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G212" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="213" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G213" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="214" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G214" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="215" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G215" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="216" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G216" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="217" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G217" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="218" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G218" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="219" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G219" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="220" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G220" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G35" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G36" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G37" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G38" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G39" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G40" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G41" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G42" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G43" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G44" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G45" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G46" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G47" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G48" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G49" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G50" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G51" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G52" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G53" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G54" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G55" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G56" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G57" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G58" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G59" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G60" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G61" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G62" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G63" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G64" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G65" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G66" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G67" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G68" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G69" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G70" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G71" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G72" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G73" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G74" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G75" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G76" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G77" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G78" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G79" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G80" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G81" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G82" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G83" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G84" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G85" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G86" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G87" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G88" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G89" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G90" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G91" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G92" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G93" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G94" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G95" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G96" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G97" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G98" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G99" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G100" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G101" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G102" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G103" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G104" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G105" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G106" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G107" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G108" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G109" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G110" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G111" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G112" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G113" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G114" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G115" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G116" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G117" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G118" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G119" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G120" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G121" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G122" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G123" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G124" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G125" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G126" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G127" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G128" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G129" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G130" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G131" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G132" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G133" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G134" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G135" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G136" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G137" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G138" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G139" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G140" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G141" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G142" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G143" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G144" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G145" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G146" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G147" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G148" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G149" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G150" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G151" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G152" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G153" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G154" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G155" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G156" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G157" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G158" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G159" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G160" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G161" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G162" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G163" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G164" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G165" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G166" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G167" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G168" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G169" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G170" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G171" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G172" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G173" s="4" t="s">
+    <row r="221" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G221" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="222" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G222" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="223" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G223" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="224" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G224" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="225" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G225" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="226" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G226" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="227" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G227" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="228" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G228" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="229" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G229" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="230" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G230" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="231" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G231" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="232" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G232" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="233" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G233" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G174" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G175" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G176" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G177" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G178" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G179" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G180" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G181" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G182" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G183" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G184" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G185" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G186" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G187" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G188" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G189" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G190" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G191" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G192" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G193" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G194" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G195" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G196" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G197" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G198" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G199" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G200" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G201" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G202" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G203" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G204" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G205" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G206" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G207" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G208" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G209" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G210" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G211" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G212" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G213" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G214" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G215" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G216" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G217" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G218" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G219" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G220" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G221" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G222" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G223" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G224" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G225" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G226" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G227" s="4" t="s">
+    <row r="234" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G234" s="3" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G228" s="4" t="s">
+    <row r="235" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G235" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G229" s="4" t="s">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G236" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G230" s="4" t="s">
+    <row r="237" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G237" s="3" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G231" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G232" s="4" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G233" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G234" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G235" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G236" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G237" s="4" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3169,6 +3084,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100203199D83812C2499E49CC0C3E7DE06C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2f8823872235ddf1d1c55d8837f3ca9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="631437c1-70b7-41ea-97e4-3973abe7cce0" xmlns:ns4="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="116abd7a6875440f2166ad9e25254cea" ns3:_="" ns4:_="">
     <xsd:import namespace="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
@@ -3377,7 +3298,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3386,13 +3307,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F8F7E8B-C071-4DC9-A2E9-BDAF31C19E75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{214CF277-9889-499D-8A02-51B999F78EC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3411,27 +3343,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82BBF237-B8F1-4EDE-B989-1271C5E3C0CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F8F7E8B-C071-4DC9-A2E9-BDAF31C19E75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="631437c1-70b7-41ea-97e4-3973abe7cce0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b5aaafdd-65a0-4d08-a467-5dbeb32cdf1b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>